<commit_message>
Removed the unnecessary Track Loss systematic for the asymmetry
</commit_message>
<xml_diff>
--- a/Sheets/DiJet-EEWW.xlsx
+++ b/Sheets/DiJet-EEWW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/Run15/DijetAsymmetryAnalysis/DijetALLCode/Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BEC2C7-D941-0F43-943E-DA1AD0583B06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A237987F-CA01-074F-A168-3E462611B2E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24000" yWindow="-20400" windowWidth="24000" windowHeight="38400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24000" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scale - EEWW" sheetId="12" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>ALL</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>4% track loss</t>
-  </si>
-  <si>
-    <t>4% Track Loss</t>
   </si>
   <si>
     <t>Best Fit</t>
@@ -185,11 +182,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000000E+00"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="170" formatCode="0.0000"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -900,7 +898,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -997,6 +995,7 @@
     <xf numFmtId="11" fontId="1" fillId="10" borderId="0" xfId="388" applyNumberFormat="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="386" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1012,7 +1011,7 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="391" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="392">
     <cellStyle name="20% - Accent2" xfId="388" builtinId="34"/>
@@ -1752,8 +1751,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F10"/>
+    <sheetView showRuler="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1769,51 +1768,51 @@
   <sheetData>
     <row r="1" spans="1:19" ht="26">
       <c r="A1" s="29"/>
-      <c r="B1" s="62" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
+      <c r="B1" s="63" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
       <c r="R1" s="29"/>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="29"/>
       <c r="B2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>33</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>34</v>
       </c>
       <c r="J2" s="12" t="s">
         <v>3</v>
@@ -1834,7 +1833,7 @@
         <v>10</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>11</v>
@@ -1844,7 +1843,7 @@
     <row r="3" spans="1:19">
       <c r="A3" s="29"/>
       <c r="B3" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="44">
         <v>15.4</v>
@@ -1875,7 +1874,7 @@
     <row r="4" spans="1:19">
       <c r="A4" s="29"/>
       <c r="B4" s="58" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="40">
         <v>18.010000000000002</v>
@@ -1918,7 +1917,7 @@
         <f t="shared" ref="N4:N10" si="4">SQRT((I4-H4)^2 + 0)</f>
         <v>0.22660000000000124</v>
       </c>
-      <c r="O4" s="65">
+      <c r="O4" s="60">
         <v>-0.21049100000000001</v>
       </c>
       <c r="P4" s="49">
@@ -1934,7 +1933,7 @@
     <row r="5" spans="1:19">
       <c r="A5" s="29"/>
       <c r="B5" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="40">
         <v>20.83</v>
@@ -1977,7 +1976,7 @@
         <f t="shared" si="4"/>
         <v>0.38749999999999929</v>
       </c>
-      <c r="O5" s="65">
+      <c r="O5" s="60">
         <v>-0.206182</v>
       </c>
       <c r="P5" s="49">
@@ -1993,7 +1992,7 @@
     <row r="6" spans="1:19">
       <c r="A6" s="29"/>
       <c r="B6" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="40">
         <v>25.14</v>
@@ -2036,7 +2035,7 @@
         <f t="shared" si="4"/>
         <v>0.39770000000000039</v>
       </c>
-      <c r="O6" s="65">
+      <c r="O6" s="60">
         <v>-0.18918599999999999</v>
       </c>
       <c r="P6" s="49">
@@ -2052,7 +2051,7 @@
     <row r="7" spans="1:19">
       <c r="A7" s="29"/>
       <c r="B7" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="40">
         <v>30.44</v>
@@ -2095,7 +2094,7 @@
         <f t="shared" si="4"/>
         <v>0.46330000000000382</v>
       </c>
-      <c r="O7" s="65">
+      <c r="O7" s="60">
         <v>-0.20305300000000001</v>
       </c>
       <c r="P7" s="49">
@@ -2111,7 +2110,7 @@
     <row r="8" spans="1:19">
       <c r="A8" s="29"/>
       <c r="B8" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="40">
         <v>36.799999999999997</v>
@@ -2154,7 +2153,7 @@
         <f t="shared" si="4"/>
         <v>0.53979999999999961</v>
       </c>
-      <c r="O8" s="65">
+      <c r="O8" s="60">
         <v>-0.20116000000000001</v>
       </c>
       <c r="P8" s="49">
@@ -2170,7 +2169,7 @@
     <row r="9" spans="1:19">
       <c r="A9" s="29"/>
       <c r="B9" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="40">
         <v>46.1</v>
@@ -2213,7 +2212,7 @@
         <f t="shared" si="4"/>
         <v>0.56380000000000052</v>
       </c>
-      <c r="O9" s="65">
+      <c r="O9" s="60">
         <v>-0.20277600000000001</v>
       </c>
       <c r="P9" s="49">
@@ -2229,7 +2228,7 @@
     <row r="10" spans="1:19">
       <c r="A10" s="29"/>
       <c r="B10" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="40">
         <v>64.040000000000006</v>
@@ -2272,7 +2271,7 @@
         <f t="shared" si="4"/>
         <v>0.66270000000000095</v>
       </c>
-      <c r="O10" s="65">
+      <c r="O10" s="60">
         <v>-0.15728600000000001</v>
       </c>
       <c r="P10" s="49">
@@ -2347,10 +2346,10 @@
       <c r="S13" s="3"/>
     </row>
     <row r="14" spans="1:19">
-      <c r="B14" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="61"/>
+      <c r="B14" s="61" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="62"/>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
@@ -2368,7 +2367,7 @@
     </row>
     <row r="15" spans="1:19">
       <c r="B15" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="13">
         <v>0.01</v>
@@ -2377,7 +2376,7 @@
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
       <c r="H15" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I15" s="22"/>
       <c r="J15" s="21"/>
@@ -2392,7 +2391,7 @@
     </row>
     <row r="16" spans="1:19">
       <c r="B16" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="13">
         <v>1.1628000000000001</v>
@@ -2414,7 +2413,7 @@
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="13">
         <v>0.81</v>
@@ -2436,7 +2435,7 @@
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="13">
         <v>0.72</v>
@@ -2445,7 +2444,7 @@
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="13">
         <v>0.32</v>
@@ -2459,7 +2458,7 @@
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="13">
         <v>0.06</v>
@@ -2467,7 +2466,7 @@
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="13">
         <v>3.2000000000000001E-2</v>
@@ -2476,7 +2475,7 @@
     </row>
     <row r="22" spans="2:19" ht="17" thickBot="1">
       <c r="B22" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="14">
         <v>0.01</v>
@@ -2542,56 +2541,55 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AW25"/>
+  <dimension ref="A1:AV25"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4:O10"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="13" width="16" customWidth="1"/>
-    <col min="14" max="18" width="13.83203125" customWidth="1"/>
-    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="23" width="13.83203125" customWidth="1"/>
-    <col min="24" max="24" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.1640625" customWidth="1"/>
-    <col min="26" max="26" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.1640625" style="2" customWidth="1"/>
-    <col min="32" max="32" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="16" customWidth="1"/>
+    <col min="13" max="17" width="13.83203125" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="13.83203125" customWidth="1"/>
+    <col min="23" max="23" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.1640625" customWidth="1"/>
+    <col min="25" max="25" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.1640625" style="2" customWidth="1"/>
+    <col min="31" max="31" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="22" customHeight="1">
+    <row r="1" spans="1:31" ht="22" customHeight="1">
       <c r="A1" s="29"/>
-      <c r="B1" s="64" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="29"/>
+      <c r="B1" s="65" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-    </row>
-    <row r="2" spans="1:32" ht="22" customHeight="1">
+    </row>
+    <row r="2" spans="1:31" ht="22" customHeight="1">
       <c r="A2" s="29"/>
       <c r="B2" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>0</v>
@@ -2600,68 +2598,64 @@
         <v>1</v>
       </c>
       <c r="E2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>4</v>
-      </c>
       <c r="G2" s="18" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="J2" s="18" t="s">
         <v>45</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="6"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-    </row>
-    <row r="3" spans="1:32" ht="22" customHeight="1">
+    </row>
+    <row r="3" spans="1:31" ht="22" customHeight="1">
       <c r="A3" s="29"/>
       <c r="B3" s="43"/>
       <c r="C3" s="51"/>
       <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
       <c r="G3" s="52"/>
       <c r="H3" s="52"/>
       <c r="I3" s="52"/>
       <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="P3" s="5"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="5"/>
+      <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="3"/>
-      <c r="AF3" s="2"/>
-    </row>
-    <row r="4" spans="1:32" ht="22" customHeight="1">
+      <c r="R3" s="5"/>
+      <c r="S3" s="3"/>
+      <c r="AE3" s="2"/>
+    </row>
+    <row r="4" spans="1:31" ht="22" customHeight="1">
       <c r="A4" s="29"/>
       <c r="B4" s="58" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="50">
         <v>8.2240000000000004E-3</v>
@@ -2669,52 +2663,49 @@
       <c r="D4" s="38">
         <v>3.565E-3</v>
       </c>
-      <c r="E4" s="38">
-        <v>2.0244499999999999E-4</v>
-      </c>
-      <c r="F4" s="50">
+      <c r="E4" s="50">
         <v>1.75431E-3</v>
       </c>
+      <c r="F4" s="38">
+        <v>4.8046100000000001E-4</v>
+      </c>
       <c r="G4" s="38">
-        <v>4.8046100000000001E-4</v>
+        <v>6.5789699999999995E-4</v>
       </c>
       <c r="H4" s="38">
-        <v>6.5789699999999995E-4</v>
-      </c>
-      <c r="I4" s="38">
-        <v>5.1137899999999997E-5</v>
-      </c>
-      <c r="J4" s="56">
+        <v>5.1137899999999996E-4</v>
+      </c>
+      <c r="I4" s="56">
         <v>0.99982599999999999</v>
       </c>
-      <c r="K4" s="59">
-        <f>((1/J4)-1)*M4</f>
+      <c r="J4" s="59">
+        <f>((1/I4)-1)*L4</f>
         <v>1.1259219704228761E-6</v>
       </c>
-      <c r="L4" s="17">
-        <f>SQRT(I4^2 +H4^2 + E4^2 +G4^2 +K4^2)</f>
-        <v>8.4099439098705845E-4</v>
-      </c>
-      <c r="M4" s="57">
-        <f t="shared" ref="M4:M10" si="0">C4-(F4)</f>
+      <c r="K4" s="17">
+        <f>SQRT(H4^2 +G4^2 +F4^2 +J4^2)</f>
+        <v>9.6186328782799655E-4</v>
+      </c>
+      <c r="L4" s="57">
+        <f>C4-(E4)</f>
         <v>6.4696900000000002E-3</v>
       </c>
-      <c r="N4" s="37"/>
-      <c r="O4" s="7">
-        <f>SQRT(L4*L4+F$13*F$13)</f>
-        <v>1.0941990521252034E-3</v>
-      </c>
-      <c r="P4" s="5"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="66">
+        <f>SQRT(K4*K4+E$13*E$13)</f>
+        <v>1.1896137963521116E-3</v>
+      </c>
+      <c r="O4" s="5"/>
+      <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="3"/>
-      <c r="AF4" s="2"/>
-    </row>
-    <row r="5" spans="1:32" ht="22" customHeight="1">
+      <c r="R4" s="5"/>
+      <c r="S4" s="3"/>
+      <c r="AE4" s="2"/>
+    </row>
+    <row r="5" spans="1:31" ht="22" customHeight="1">
       <c r="A5" s="29"/>
       <c r="B5" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="50">
         <v>5.4010000000000004E-3</v>
@@ -2722,52 +2713,49 @@
       <c r="D5" s="38">
         <v>2.7650000000000001E-3</v>
       </c>
-      <c r="E5" s="38">
-        <v>-2.16636E-4</v>
-      </c>
-      <c r="F5" s="50">
+      <c r="E5" s="50">
         <v>1.4019E-3</v>
       </c>
+      <c r="F5" s="38">
+        <v>3.4978299999999999E-4</v>
+      </c>
       <c r="G5" s="38">
-        <v>3.4978299999999999E-4</v>
+        <v>5.4414800000000005E-4</v>
       </c>
       <c r="H5" s="38">
-        <v>5.4414800000000005E-4</v>
-      </c>
-      <c r="I5" s="38">
-        <v>5.9493300000000002E-5</v>
-      </c>
-      <c r="J5" s="56">
+        <v>5.9493299999999996E-4</v>
+      </c>
+      <c r="I5" s="56">
         <v>0.999838</v>
       </c>
-      <c r="K5" s="59">
-        <f t="shared" ref="K5:K10" si="1">((1/J5)-1)*M5</f>
+      <c r="J5" s="59">
+        <f t="shared" ref="J5:J10" si="0">((1/I5)-1)*L5</f>
         <v>6.4795916938550861E-7</v>
       </c>
-      <c r="L5" s="17">
-        <f t="shared" ref="L5:L10" si="2">SQRT(I5^2 +H5^2 + E5^2 +G5^2 +K5^2)</f>
-        <v>6.8477457756912618E-4</v>
-      </c>
-      <c r="M5" s="57">
-        <f t="shared" si="0"/>
+      <c r="K5" s="17">
+        <f t="shared" ref="K5:K10" si="1">SQRT(H5^2 +G5^2 +F5^2 +J5^2)</f>
+        <v>8.7885771734285019E-4</v>
+      </c>
+      <c r="L5" s="57">
+        <f>C5-(E5)</f>
         <v>3.9991000000000002E-3</v>
       </c>
-      <c r="N5" s="37"/>
-      <c r="O5" s="7">
-        <f t="shared" ref="O5:O10" si="3">SQRT(L5*L5+F$13*F$13)</f>
-        <v>9.7924267783066677E-4</v>
-      </c>
-      <c r="P5" s="5"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="66">
+        <f t="shared" ref="N5:N10" si="2">SQRT(K5*K5+E$13*E$13)</f>
+        <v>1.1235616971635716E-3</v>
+      </c>
+      <c r="O5" s="5"/>
+      <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="3"/>
-      <c r="AF5" s="2"/>
-    </row>
-    <row r="6" spans="1:32" ht="22" customHeight="1">
+      <c r="R5" s="5"/>
+      <c r="S5" s="3"/>
+      <c r="AE5" s="2"/>
+    </row>
+    <row r="6" spans="1:31" ht="22" customHeight="1">
       <c r="A6" s="29"/>
       <c r="B6" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="50">
         <v>1.5969999999999999E-3</v>
@@ -2775,52 +2763,49 @@
       <c r="D6" s="38">
         <v>3.4610000000000001E-3</v>
       </c>
-      <c r="E6" s="38">
-        <v>-2.94682E-4</v>
-      </c>
-      <c r="F6" s="50">
+      <c r="E6" s="50">
         <v>1.05937E-3</v>
       </c>
+      <c r="F6" s="38">
+        <v>4.7445000000000001E-4</v>
+      </c>
       <c r="G6" s="38">
-        <v>4.7445000000000001E-4</v>
+        <v>4.54408E-4</v>
       </c>
       <c r="H6" s="38">
-        <v>4.54408E-4</v>
-      </c>
-      <c r="I6" s="38">
-        <v>8.2136200000000001E-5</v>
-      </c>
-      <c r="J6" s="56">
+        <v>8.2136199999999996E-4</v>
+      </c>
+      <c r="I6" s="56">
         <v>0.99704400000000004</v>
       </c>
-      <c r="K6" s="59">
+      <c r="J6" s="59">
+        <f t="shared" si="0"/>
+        <v>1.593945984329607E-6</v>
+      </c>
+      <c r="K6" s="17">
         <f t="shared" si="1"/>
-        <v>1.593945984329607E-6</v>
-      </c>
-      <c r="L6" s="17">
+        <v>1.0517735063557178E-3</v>
+      </c>
+      <c r="L6" s="57">
+        <f>C6-(E6)</f>
+        <v>5.3762999999999988E-4</v>
+      </c>
+      <c r="M6" s="37"/>
+      <c r="N6" s="66">
         <f t="shared" si="2"/>
-        <v>7.2469014765087086E-4</v>
-      </c>
-      <c r="M6" s="57">
-        <f t="shared" si="0"/>
-        <v>5.3762999999999988E-4</v>
-      </c>
-      <c r="N6" s="37"/>
-      <c r="O6" s="7">
-        <f t="shared" si="3"/>
-        <v>1.0075593332912166E-3</v>
-      </c>
-      <c r="P6" s="5"/>
+        <v>1.2634189759030063E-3</v>
+      </c>
+      <c r="O6" s="5"/>
+      <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="3"/>
-      <c r="AF6" s="2"/>
-    </row>
-    <row r="7" spans="1:32" ht="22" customHeight="1">
+      <c r="R6" s="5"/>
+      <c r="S6" s="3"/>
+      <c r="AE6" s="2"/>
+    </row>
+    <row r="7" spans="1:31" ht="22" customHeight="1">
       <c r="A7" s="29"/>
       <c r="B7" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="50">
         <v>1.3690000000000001E-2</v>
@@ -2828,52 +2813,49 @@
       <c r="D7" s="38">
         <v>5.0600000000000003E-3</v>
       </c>
-      <c r="E7" s="38">
-        <v>-1.5015699999999999E-4</v>
-      </c>
-      <c r="F7" s="50">
+      <c r="E7" s="50">
         <v>1.5485900000000001E-3</v>
       </c>
+      <c r="F7" s="38">
+        <v>6.6018700000000001E-4</v>
+      </c>
       <c r="G7" s="38">
-        <v>6.6018700000000001E-4</v>
+        <v>3.7832300000000002E-4</v>
       </c>
       <c r="H7" s="38">
-        <v>3.7832300000000002E-4</v>
-      </c>
-      <c r="I7" s="38">
-        <v>1.06012E-4</v>
-      </c>
-      <c r="J7" s="56">
+        <v>1.0601199999999999E-3</v>
+      </c>
+      <c r="I7" s="56">
         <v>0.99734500000000004</v>
       </c>
-      <c r="K7" s="59">
+      <c r="J7" s="59">
+        <f t="shared" si="0"/>
+        <v>3.2321256485970921E-5</v>
+      </c>
+      <c r="K7" s="17">
         <f t="shared" si="1"/>
-        <v>3.2321256485970921E-5</v>
-      </c>
-      <c r="L7" s="17">
+        <v>1.3053253407939462E-3</v>
+      </c>
+      <c r="L7" s="57">
+        <f>C7-(E7)</f>
+        <v>1.214141E-2</v>
+      </c>
+      <c r="M7" s="37"/>
+      <c r="N7" s="66">
         <f t="shared" si="2"/>
-        <v>7.834574013383446E-4</v>
-      </c>
-      <c r="M7" s="57">
-        <f t="shared" si="0"/>
-        <v>1.214141E-2</v>
-      </c>
-      <c r="N7" s="37"/>
-      <c r="O7" s="7">
-        <f t="shared" si="3"/>
-        <v>1.0506214826053349E-3</v>
-      </c>
-      <c r="P7" s="5"/>
+        <v>1.4811732664745309E-3</v>
+      </c>
+      <c r="O7" s="5"/>
+      <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="3"/>
-      <c r="AF7" s="2"/>
-    </row>
-    <row r="8" spans="1:32" ht="22" customHeight="1">
+      <c r="R7" s="5"/>
+      <c r="S7" s="3"/>
+      <c r="AE7" s="2"/>
+    </row>
+    <row r="8" spans="1:31" ht="22" customHeight="1">
       <c r="A8" s="29"/>
       <c r="B8" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="50">
         <v>3.0051000000000001E-2</v>
@@ -2881,52 +2863,49 @@
       <c r="D8" s="38">
         <v>8.1089999999999999E-3</v>
       </c>
-      <c r="E8" s="38">
-        <v>5.1619799999999997E-5</v>
-      </c>
-      <c r="F8" s="50">
+      <c r="E8" s="50">
         <v>4.4516899999999998E-4</v>
       </c>
+      <c r="F8" s="38">
+        <v>9.2922000000000002E-4</v>
+      </c>
       <c r="G8" s="38">
-        <v>9.2922000000000002E-4</v>
+        <v>3.2183299999999999E-4</v>
       </c>
       <c r="H8" s="38">
-        <v>3.2183299999999999E-4</v>
-      </c>
-      <c r="I8" s="38">
-        <v>1.1896399999999999E-4</v>
-      </c>
-      <c r="J8" s="56">
+        <v>1.1896400000000001E-3</v>
+      </c>
+      <c r="I8" s="56">
         <v>0.999973</v>
       </c>
-      <c r="K8" s="59">
+      <c r="J8" s="59">
+        <f t="shared" si="0"/>
+        <v>7.9937902023500256E-7</v>
+      </c>
+      <c r="K8" s="17">
         <f t="shared" si="1"/>
-        <v>7.9937902023500256E-7</v>
-      </c>
-      <c r="L8" s="17">
+        <v>1.5434604811577842E-3</v>
+      </c>
+      <c r="L8" s="57">
+        <f>C8-(E8)</f>
+        <v>2.9605831000000003E-2</v>
+      </c>
+      <c r="M8" s="37"/>
+      <c r="N8" s="66">
         <f t="shared" si="2"/>
-        <v>9.9188908873112328E-4</v>
-      </c>
-      <c r="M8" s="57">
-        <f t="shared" si="0"/>
-        <v>2.9605831000000003E-2</v>
-      </c>
-      <c r="N8" s="37"/>
-      <c r="O8" s="7">
-        <f t="shared" si="3"/>
-        <v>1.2140197545113746E-3</v>
-      </c>
-      <c r="P8" s="5"/>
+        <v>1.6947773472925046E-3</v>
+      </c>
+      <c r="O8" s="5"/>
+      <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="3"/>
-      <c r="AF8" s="2"/>
-    </row>
-    <row r="9" spans="1:32" ht="22" customHeight="1">
+      <c r="R8" s="5"/>
+      <c r="S8" s="3"/>
+      <c r="AE8" s="2"/>
+    </row>
+    <row r="9" spans="1:31" ht="22" customHeight="1">
       <c r="A9" s="29"/>
       <c r="B9" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="50">
         <v>2.0045E-2</v>
@@ -2934,52 +2913,49 @@
       <c r="D9" s="38">
         <v>1.2102999999999999E-2</v>
       </c>
-      <c r="E9" s="38">
-        <v>1.5549300000000001E-4</v>
-      </c>
-      <c r="F9" s="50">
+      <c r="E9" s="50">
         <v>-5.3214199999999999E-4</v>
       </c>
+      <c r="F9" s="38">
+        <v>1.03648E-3</v>
+      </c>
       <c r="G9" s="38">
-        <v>1.03648E-3</v>
+        <v>2.7361900000000001E-4</v>
       </c>
       <c r="H9" s="38">
-        <v>2.7361900000000001E-4</v>
-      </c>
-      <c r="I9" s="38">
-        <v>1.7333600000000001E-4</v>
-      </c>
-      <c r="J9" s="56">
+        <v>1.73336E-3</v>
+      </c>
+      <c r="I9" s="56">
         <v>0.999969</v>
       </c>
-      <c r="K9" s="59">
+      <c r="J9" s="59">
+        <f t="shared" si="0"/>
+        <v>6.3791117724695982E-7</v>
+      </c>
+      <c r="K9" s="17">
         <f t="shared" si="1"/>
-        <v>6.3791117724695982E-7</v>
-      </c>
-      <c r="L9" s="17">
+        <v>2.0380616879995734E-3</v>
+      </c>
+      <c r="L9" s="57">
+        <f>C9-(E9)</f>
+        <v>2.0577142E-2</v>
+      </c>
+      <c r="M9" s="37"/>
+      <c r="N9" s="66">
         <f t="shared" si="2"/>
-        <v>1.0969876920169479E-3</v>
-      </c>
-      <c r="M9" s="57">
-        <f t="shared" si="0"/>
-        <v>2.0577142E-2</v>
-      </c>
-      <c r="N9" s="37"/>
-      <c r="O9" s="7">
-        <f t="shared" si="3"/>
-        <v>1.30130011774251E-3</v>
-      </c>
-      <c r="P9" s="5"/>
+        <v>2.1549235355556519E-3</v>
+      </c>
+      <c r="O9" s="5"/>
+      <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="3"/>
-      <c r="AF9" s="2"/>
-    </row>
-    <row r="10" spans="1:32" ht="22" customHeight="1">
+      <c r="R9" s="5"/>
+      <c r="S9" s="3"/>
+      <c r="AE9" s="2"/>
+    </row>
+    <row r="10" spans="1:31" ht="22" customHeight="1">
       <c r="A10" s="29"/>
       <c r="B10" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="50">
         <v>1.3653E-2</v>
@@ -2987,199 +2963,191 @@
       <c r="D10" s="38">
         <v>4.1832000000000001E-2</v>
       </c>
-      <c r="E10" s="38">
-        <v>1.8350800000000001E-4</v>
-      </c>
-      <c r="F10" s="50">
+      <c r="E10" s="50">
         <v>-5.8756199999999998E-3</v>
       </c>
+      <c r="F10" s="38">
+        <v>2.12853E-3</v>
+      </c>
       <c r="G10" s="38">
-        <v>2.12853E-3</v>
+        <v>2.3663800000000001E-4</v>
       </c>
       <c r="H10" s="38">
-        <v>2.3663800000000001E-4</v>
-      </c>
-      <c r="I10" s="38">
-        <v>3.3045600000000002E-4</v>
-      </c>
-      <c r="J10" s="56">
+        <v>3.3045599999999998E-3</v>
+      </c>
+      <c r="I10" s="56">
         <v>1</v>
       </c>
-      <c r="K10" s="59">
+      <c r="J10" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="17">
+        <v>3.9378616402235365E-3</v>
+      </c>
+      <c r="L10" s="57">
+        <f>C10-(E10)</f>
+        <v>1.952862E-2</v>
+      </c>
+      <c r="M10" s="37"/>
+      <c r="N10" s="66">
         <f t="shared" si="2"/>
-        <v>2.1747445500435217E-3</v>
-      </c>
-      <c r="M10" s="57">
-        <f t="shared" si="0"/>
-        <v>1.952862E-2</v>
-      </c>
-      <c r="N10" s="37"/>
-      <c r="O10" s="7">
-        <f t="shared" si="3"/>
-        <v>2.2846255399833031E-3</v>
-      </c>
-      <c r="P10" s="5"/>
+        <v>3.999594266615553E-3</v>
+      </c>
+      <c r="O10" s="5"/>
+      <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="3"/>
-      <c r="AF10" s="2"/>
-    </row>
-    <row r="11" spans="1:32" ht="22" customHeight="1">
+      <c r="R10" s="5"/>
+      <c r="S10" s="3"/>
+      <c r="AE10" s="2"/>
+    </row>
+    <row r="11" spans="1:31" ht="22" customHeight="1">
       <c r="A11" s="29"/>
       <c r="B11" s="43"/>
       <c r="C11" s="51"/>
       <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="52"/>
       <c r="G11" s="52"/>
       <c r="H11" s="52"/>
       <c r="I11" s="52"/>
       <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="55"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="5"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="3"/>
-      <c r="AF11" s="2"/>
-    </row>
-    <row r="12" spans="1:32" ht="22" customHeight="1" thickBot="1">
+      <c r="R11" s="5"/>
+      <c r="S11" s="3"/>
+      <c r="AE11" s="2"/>
+    </row>
+    <row r="12" spans="1:31" ht="22" customHeight="1" thickBot="1">
       <c r="A12" s="29"/>
       <c r="B12" s="30"/>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="35"/>
       <c r="G12" s="35"/>
       <c r="H12" s="35"/>
       <c r="I12" s="35"/>
       <c r="J12" s="35"/>
       <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="5"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="3"/>
-      <c r="AF12" s="2"/>
-    </row>
-    <row r="13" spans="1:32" ht="22" customHeight="1" thickBot="1">
+      <c r="R12" s="5"/>
+      <c r="S12" s="3"/>
+      <c r="AE12" s="2"/>
+    </row>
+    <row r="13" spans="1:31" ht="22" customHeight="1" thickBot="1">
       <c r="B13" s="19"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="41" t="s">
+      <c r="C13" s="34"/>
+      <c r="D13" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="42">
+      <c r="E13" s="42">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="G13" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" s="35"/>
+      <c r="F13" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="35"/>
+      <c r="H13" s="25"/>
       <c r="I13" s="25"/>
       <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="5"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="3"/>
-      <c r="AF13" s="2"/>
-    </row>
-    <row r="14" spans="1:32" ht="22" customHeight="1">
+      <c r="R13" s="5"/>
+      <c r="S13" s="3"/>
+      <c r="AE13" s="2"/>
+    </row>
+    <row r="14" spans="1:31" ht="22" customHeight="1">
       <c r="B14" s="19"/>
-      <c r="C14" s="24"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="34"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="35"/>
       <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
+      <c r="H14" s="25"/>
       <c r="I14" s="25"/>
       <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="5"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="3"/>
-      <c r="AF14" s="2"/>
-    </row>
-    <row r="15" spans="1:32" ht="22" customHeight="1">
+      <c r="R14" s="5"/>
+      <c r="S14" s="3"/>
+      <c r="AE14" s="2"/>
+    </row>
+    <row r="15" spans="1:31" ht="22" customHeight="1">
       <c r="B15" s="19"/>
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="25"/>
       <c r="G15" s="25"/>
       <c r="H15" s="25"/>
       <c r="I15" s="25"/>
       <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="5"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="3"/>
-      <c r="AF15" s="2"/>
-    </row>
-    <row r="16" spans="1:32" ht="22" customHeight="1">
+      <c r="R15" s="5"/>
+      <c r="S15" s="3"/>
+      <c r="AE15" s="2"/>
+    </row>
+    <row r="16" spans="1:31" ht="22" customHeight="1">
       <c r="B16" s="19"/>
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="25"/>
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
       <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="5"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="3"/>
-      <c r="AF16" s="2"/>
-    </row>
-    <row r="18" spans="4:49">
+      <c r="R16" s="5"/>
+      <c r="S16" s="3"/>
+      <c r="AE16" s="2"/>
+    </row>
+    <row r="18" spans="4:48">
+      <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="4:49">
+    </row>
+    <row r="19" spans="4:48">
+      <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-    </row>
-    <row r="20" spans="4:49">
+    </row>
+    <row r="20" spans="4:48">
+      <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -3201,7 +3169,7 @@
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
+      <c r="AF20" s="1"/>
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
@@ -3218,9 +3186,8 @@
       <c r="AT20" s="1"/>
       <c r="AU20" s="1"/>
       <c r="AV20" s="1"/>
-      <c r="AW20" s="1"/>
-    </row>
-    <row r="21" spans="4:49">
+    </row>
+    <row r="21" spans="4:48">
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -3243,9 +3210,8 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-    </row>
-    <row r="22" spans="4:49">
+    </row>
+    <row r="22" spans="4:48">
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -3268,16 +3234,15 @@
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
+      <c r="AE22" s="1"/>
       <c r="AF22" s="1"/>
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
-      <c r="AL22" s="1"/>
-    </row>
-    <row r="23" spans="4:49">
+    </row>
+    <row r="23" spans="4:48">
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -3303,10 +3268,10 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
-      <c r="AC23" s="1"/>
-      <c r="AF23" s="1"/>
-    </row>
-    <row r="24" spans="4:49">
+      <c r="AE23" s="1"/>
+    </row>
+    <row r="24" spans="4:48">
+      <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -3330,9 +3295,9 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
-      <c r="AC24" s="1"/>
-    </row>
-    <row r="25" spans="4:49">
+    </row>
+    <row r="25" spans="4:48">
+      <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -3355,11 +3320,10 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
-      <c r="AB25" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B1:L1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Update Parton Mass Shift to remove the UE correction
</commit_message>
<xml_diff>
--- a/Sheets/DiJet-EEWW.xlsx
+++ b/Sheets/DiJet-EEWW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/Run15/DijetAsymmetryAnalysis/DijetALLCode/Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A237987F-CA01-074F-A168-3E462611B2E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EF8996-92AA-8E40-AB4D-5D2CBE53D15C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24000" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-20400" windowWidth="24000" windowHeight="38400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scale - EEWW" sheetId="12" r:id="rId1"/>
@@ -187,9 +187,9 @@
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0000E+00"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -270,6 +270,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -898,7 +904,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -996,6 +1002,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="386" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1011,7 +1018,8 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="391" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="388" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="392">
     <cellStyle name="20% - Accent2" xfId="388" builtinId="34"/>
@@ -1751,8 +1759,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1768,24 +1776,24 @@
   <sheetData>
     <row r="1" spans="1:19" ht="26">
       <c r="A1" s="29"/>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="64"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
       <c r="R1" s="29"/>
     </row>
     <row r="2" spans="1:19">
@@ -1883,21 +1891,21 @@
         <v>17.93</v>
       </c>
       <c r="E4" s="40">
-        <v>18.7438</v>
+        <v>20.2897</v>
       </c>
       <c r="F4" s="39">
         <v>17.93</v>
       </c>
       <c r="G4" s="39">
-        <v>18.970400000000001</v>
+        <v>20.4862</v>
       </c>
       <c r="H4" s="9">
         <f t="shared" ref="H4:H10" si="0">G4</f>
-        <v>18.970400000000001</v>
+        <v>20.4862</v>
       </c>
       <c r="I4" s="9">
         <f t="shared" ref="I4:I10" si="1">E4</f>
-        <v>18.7438</v>
+        <v>20.2897</v>
       </c>
       <c r="J4" s="39">
         <v>0.457569</v>
@@ -1907,15 +1915,15 @@
       </c>
       <c r="L4" s="9">
         <f t="shared" ref="L4:L10" si="2">I4*SQRT(((1-J4)*$C$15)^2+((1-J4)*((C$16-C$17*C$18)*C$19*C$20/C$17))^2)</f>
-        <v>0.17276822162107214</v>
+        <v>0.18701732766168372</v>
       </c>
       <c r="M4" s="9">
         <f t="shared" ref="M4:M10" si="3">I4*J4*SQRT(C$21^2+C$22^2)</f>
-        <v>0.28753941897807683</v>
+        <v>0.31125431071818338</v>
       </c>
       <c r="N4" s="9">
         <f t="shared" ref="N4:N10" si="4">SQRT((I4-H4)^2 + 0)</f>
-        <v>0.22660000000000124</v>
+        <v>0.19650000000000034</v>
       </c>
       <c r="O4" s="60">
         <v>-0.21049100000000001</v>
@@ -1925,7 +1933,7 @@
       </c>
       <c r="Q4" s="10">
         <f>SQRT(K4^2+L4^2+M4^2+N4^2+O4^2+P4^2)</f>
-        <v>0.52318882123848798</v>
+        <v>0.52945083207690702</v>
       </c>
       <c r="R4" s="29"/>
       <c r="S4" s="3"/>
@@ -1942,21 +1950,21 @@
         <v>20.47</v>
       </c>
       <c r="E5" s="40">
-        <v>21.958200000000001</v>
+        <v>23.497199999999999</v>
       </c>
       <c r="F5" s="39">
         <v>20.46</v>
       </c>
       <c r="G5" s="39">
-        <v>22.345700000000001</v>
+        <v>23.849699999999999</v>
       </c>
       <c r="H5" s="9">
         <f t="shared" si="0"/>
-        <v>22.345700000000001</v>
+        <v>23.849699999999999</v>
       </c>
       <c r="I5" s="9">
         <f t="shared" si="1"/>
-        <v>21.958200000000001</v>
+        <v>23.497199999999999</v>
       </c>
       <c r="J5" s="39">
         <v>0.43835200000000002</v>
@@ -1966,15 +1974,15 @@
       </c>
       <c r="L5" s="9">
         <f t="shared" si="2"/>
-        <v>0.20956689212734306</v>
+        <v>0.22425495613003821</v>
       </c>
       <c r="M5" s="9">
         <f t="shared" si="3"/>
-        <v>0.32270291200754325</v>
+        <v>0.34532042080059594</v>
       </c>
       <c r="N5" s="9">
         <f t="shared" si="4"/>
-        <v>0.38749999999999929</v>
+        <v>0.35249999999999915</v>
       </c>
       <c r="O5" s="60">
         <v>-0.206182</v>
@@ -1984,7 +1992,7 @@
       </c>
       <c r="Q5" s="10">
         <f t="shared" ref="Q5:Q10" si="5">SQRT(K5^2+L5^2+M5^2+N5^2+O5^2+P5^2)</f>
-        <v>0.611793959666178</v>
+        <v>0.60817174857168876</v>
       </c>
       <c r="R5" s="29"/>
       <c r="S5" s="3"/>
@@ -2001,21 +2009,21 @@
         <v>24.92</v>
       </c>
       <c r="E6" s="40">
-        <v>26.774000000000001</v>
+        <v>28.280899999999999</v>
       </c>
       <c r="F6" s="39">
         <v>24.91</v>
       </c>
       <c r="G6" s="39">
-        <v>27.171700000000001</v>
+        <v>28.625</v>
       </c>
       <c r="H6" s="9">
         <f t="shared" si="0"/>
-        <v>27.171700000000001</v>
+        <v>28.625</v>
       </c>
       <c r="I6" s="9">
         <f t="shared" si="1"/>
-        <v>26.774000000000001</v>
+        <v>28.280899999999999</v>
       </c>
       <c r="J6" s="39">
         <v>0.41592699999999999</v>
@@ -2025,15 +2033,15 @@
       </c>
       <c r="L6" s="9">
         <f t="shared" si="2"/>
-        <v>0.26573093113045926</v>
+        <v>0.28068685628622558</v>
       </c>
       <c r="M6" s="9">
         <f t="shared" si="3"/>
-        <v>0.37334774132152804</v>
+        <v>0.39436057882796743</v>
       </c>
       <c r="N6" s="9">
         <f t="shared" si="4"/>
-        <v>0.39770000000000039</v>
+        <v>0.34410000000000096</v>
       </c>
       <c r="O6" s="60">
         <v>-0.18918599999999999</v>
@@ -2043,7 +2051,7 @@
       </c>
       <c r="Q6" s="10">
         <f t="shared" si="5"/>
-        <v>0.66876624615357783</v>
+        <v>0.65710861028476442</v>
       </c>
       <c r="R6" s="29"/>
       <c r="S6" s="3"/>
@@ -2060,21 +2068,21 @@
         <v>29.9</v>
       </c>
       <c r="E7" s="40">
-        <v>32.680399999999999</v>
+        <v>34.152900000000002</v>
       </c>
       <c r="F7" s="39">
         <v>29.87</v>
       </c>
       <c r="G7" s="39">
-        <v>33.143700000000003</v>
+        <v>34.594700000000003</v>
       </c>
       <c r="H7" s="9">
         <f t="shared" si="0"/>
-        <v>33.143700000000003</v>
+        <v>34.594700000000003</v>
       </c>
       <c r="I7" s="9">
         <f t="shared" si="1"/>
-        <v>32.680399999999999</v>
+        <v>34.152900000000002</v>
       </c>
       <c r="J7" s="39">
         <v>0.39760200000000001</v>
@@ -2084,15 +2092,15 @@
       </c>
       <c r="L7" s="9">
         <f t="shared" si="2"/>
-        <v>0.33452810052726045</v>
+        <v>0.34960112986675423</v>
       </c>
       <c r="M7" s="9">
         <f t="shared" si="3"/>
-        <v>0.43563130332141964</v>
+        <v>0.45525979912137288</v>
       </c>
       <c r="N7" s="9">
         <f t="shared" si="4"/>
-        <v>0.46330000000000382</v>
+        <v>0.44180000000000064</v>
       </c>
       <c r="O7" s="60">
         <v>-0.20305300000000001</v>
@@ -2102,7 +2110,7 @@
       </c>
       <c r="Q7" s="10">
         <f t="shared" si="5"/>
-        <v>0.77466568485308507</v>
+        <v>0.78002950297610185</v>
       </c>
       <c r="R7" s="29"/>
       <c r="S7" s="3"/>
@@ -2119,21 +2127,21 @@
         <v>36.409999999999997</v>
       </c>
       <c r="E8" s="40">
-        <v>39.514800000000001</v>
+        <v>40.955199999999998</v>
       </c>
       <c r="F8" s="39">
         <v>36.39</v>
       </c>
       <c r="G8" s="39">
-        <v>40.054600000000001</v>
+        <v>41.461100000000002</v>
       </c>
       <c r="H8" s="9">
         <f t="shared" si="0"/>
-        <v>40.054600000000001</v>
+        <v>41.461100000000002</v>
       </c>
       <c r="I8" s="9">
         <f t="shared" si="1"/>
-        <v>39.514800000000001</v>
+        <v>40.955199999999998</v>
       </c>
       <c r="J8" s="39">
         <v>0.38540000000000002</v>
@@ -2143,15 +2151,15 @@
       </c>
       <c r="L8" s="9">
         <f t="shared" si="2"/>
-        <v>0.41268060997796968</v>
+        <v>0.42772371156553352</v>
       </c>
       <c r="M8" s="9">
         <f t="shared" si="3"/>
-        <v>0.51056924886287658</v>
+        <v>0.52918060324306027</v>
       </c>
       <c r="N8" s="9">
         <f t="shared" si="4"/>
-        <v>0.53979999999999961</v>
+        <v>0.50590000000000401</v>
       </c>
       <c r="O8" s="60">
         <v>-0.20116000000000001</v>
@@ -2161,7 +2169,7 @@
       </c>
       <c r="Q8" s="10">
         <f t="shared" si="5"/>
-        <v>0.89067972926817573</v>
+        <v>0.88873763883225354</v>
       </c>
       <c r="R8" s="29"/>
       <c r="S8" s="3"/>
@@ -2178,21 +2186,21 @@
         <v>45.77</v>
       </c>
       <c r="E9" s="40">
-        <v>49.3431</v>
+        <v>50.747900000000001</v>
       </c>
       <c r="F9" s="39">
         <v>45.71</v>
       </c>
       <c r="G9" s="39">
-        <v>49.9069</v>
+        <v>51.280999999999999</v>
       </c>
       <c r="H9" s="9">
         <f t="shared" si="0"/>
-        <v>49.9069</v>
+        <v>51.280999999999999</v>
       </c>
       <c r="I9" s="9">
         <f t="shared" si="1"/>
-        <v>49.3431</v>
+        <v>50.747900000000001</v>
       </c>
       <c r="J9" s="39">
         <v>0.37880399999999997</v>
@@ -2202,15 +2210,15 @@
       </c>
       <c r="L9" s="9">
         <f t="shared" si="2"/>
-        <v>0.52085495617039179</v>
+        <v>0.53568371728244524</v>
       </c>
       <c r="M9" s="9">
         <f t="shared" si="3"/>
-        <v>0.6266486994396111</v>
+        <v>0.64448941258841541</v>
       </c>
       <c r="N9" s="9">
         <f t="shared" si="4"/>
-        <v>0.56380000000000052</v>
+        <v>0.53309999999999746</v>
       </c>
       <c r="O9" s="60">
         <v>-0.20277600000000001</v>
@@ -2220,7 +2228,7 @@
       </c>
       <c r="Q9" s="10">
         <f t="shared" si="5"/>
-        <v>1.0237335675523478</v>
+        <v>1.0260120649178239</v>
       </c>
       <c r="R9" s="29"/>
       <c r="S9" s="3"/>
@@ -2237,21 +2245,21 @@
         <v>63.23</v>
       </c>
       <c r="E10" s="40">
-        <v>67.796400000000006</v>
+        <v>69.107900000000001</v>
       </c>
       <c r="F10" s="39">
         <v>63.17</v>
       </c>
       <c r="G10" s="39">
-        <v>68.459100000000007</v>
+        <v>69.722200000000001</v>
       </c>
       <c r="H10" s="9">
         <f t="shared" si="0"/>
-        <v>68.459100000000007</v>
+        <v>69.722200000000001</v>
       </c>
       <c r="I10" s="9">
         <f t="shared" si="1"/>
-        <v>67.796400000000006</v>
+        <v>69.107900000000001</v>
       </c>
       <c r="J10" s="39">
         <v>0.37034099999999998</v>
@@ -2261,15 +2269,15 @@
       </c>
       <c r="L10" s="9">
         <f t="shared" si="2"/>
-        <v>0.725393681573551</v>
+        <v>0.73942619382174868</v>
       </c>
       <c r="M10" s="9">
         <f t="shared" si="3"/>
-        <v>0.84176639511165652</v>
+        <v>0.85805010084218092</v>
       </c>
       <c r="N10" s="9">
         <f t="shared" si="4"/>
-        <v>0.66270000000000095</v>
+        <v>0.61430000000000007</v>
       </c>
       <c r="O10" s="60">
         <v>-0.15728600000000001</v>
@@ -2279,7 +2287,7 @@
       </c>
       <c r="Q10" s="10">
         <f t="shared" si="5"/>
-        <v>1.3158938140762366</v>
+        <v>1.310726571174551</v>
       </c>
       <c r="R10" s="29"/>
       <c r="S10" s="3"/>
@@ -2346,10 +2354,10 @@
       <c r="S13" s="3"/>
     </row>
     <row r="14" spans="1:19">
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="62"/>
+      <c r="C14" s="63"/>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
@@ -2396,8 +2404,8 @@
       <c r="C16" s="13">
         <v>1.1628000000000001</v>
       </c>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
       <c r="G16" s="21"/>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
@@ -2418,8 +2426,8 @@
       <c r="C17" s="13">
         <v>0.81</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
       <c r="G17" s="21"/>
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
@@ -2440,6 +2448,8 @@
       <c r="C18" s="13">
         <v>0.72</v>
       </c>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
       <c r="Q18" s="11"/>
     </row>
     <row r="19" spans="2:19">
@@ -2449,6 +2459,8 @@
       <c r="C19" s="13">
         <v>0.32</v>
       </c>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -2463,6 +2475,8 @@
       <c r="C20" s="13">
         <v>0.06</v>
       </c>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="15" t="s">
@@ -2471,7 +2485,8 @@
       <c r="C21" s="13">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
     </row>
     <row r="22" spans="2:19" ht="17" thickBot="1">
       <c r="B22" s="16" t="s">
@@ -2480,10 +2495,12 @@
       <c r="C22" s="14">
         <v>0.01</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
     </row>
     <row r="23" spans="2:19">
-      <c r="E23" s="4"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
     </row>
     <row r="24" spans="2:19">
       <c r="E24" s="4"/>
@@ -2543,7 +2560,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AV25"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="K4" sqref="K4:K10"/>
     </sheetView>
   </sheetViews>
@@ -2566,19 +2583,19 @@
   <sheetData>
     <row r="1" spans="1:31" ht="22" customHeight="1">
       <c r="A1" s="29"/>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
       <c r="M1" s="29"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -2687,11 +2704,11 @@
         <v>9.6186328782799655E-4</v>
       </c>
       <c r="L4" s="57">
-        <f>C4-(E4)</f>
+        <f t="shared" ref="L4:L10" si="0">C4-(E4)</f>
         <v>6.4696900000000002E-3</v>
       </c>
       <c r="M4" s="37"/>
-      <c r="N4" s="66">
+      <c r="N4" s="61">
         <f>SQRT(K4*K4+E$13*E$13)</f>
         <v>1.1896137963521116E-3</v>
       </c>
@@ -2729,20 +2746,20 @@
         <v>0.999838</v>
       </c>
       <c r="J5" s="59">
-        <f t="shared" ref="J5:J10" si="0">((1/I5)-1)*L5</f>
+        <f t="shared" ref="J5:J10" si="1">((1/I5)-1)*L5</f>
         <v>6.4795916938550861E-7</v>
       </c>
       <c r="K5" s="17">
-        <f t="shared" ref="K5:K10" si="1">SQRT(H5^2 +G5^2 +F5^2 +J5^2)</f>
+        <f t="shared" ref="K5:K10" si="2">SQRT(H5^2 +G5^2 +F5^2 +J5^2)</f>
         <v>8.7885771734285019E-4</v>
       </c>
       <c r="L5" s="57">
-        <f>C5-(E5)</f>
+        <f t="shared" si="0"/>
         <v>3.9991000000000002E-3</v>
       </c>
       <c r="M5" s="37"/>
-      <c r="N5" s="66">
-        <f t="shared" ref="N5:N10" si="2">SQRT(K5*K5+E$13*E$13)</f>
+      <c r="N5" s="61">
+        <f t="shared" ref="N5:N10" si="3">SQRT(K5*K5+E$13*E$13)</f>
         <v>1.1235616971635716E-3</v>
       </c>
       <c r="O5" s="5"/>
@@ -2779,20 +2796,20 @@
         <v>0.99704400000000004</v>
       </c>
       <c r="J6" s="59">
+        <f t="shared" si="1"/>
+        <v>1.593945984329607E-6</v>
+      </c>
+      <c r="K6" s="17">
+        <f t="shared" si="2"/>
+        <v>1.0517735063557178E-3</v>
+      </c>
+      <c r="L6" s="57">
         <f t="shared" si="0"/>
-        <v>1.593945984329607E-6</v>
-      </c>
-      <c r="K6" s="17">
-        <f t="shared" si="1"/>
-        <v>1.0517735063557178E-3</v>
-      </c>
-      <c r="L6" s="57">
-        <f>C6-(E6)</f>
         <v>5.3762999999999988E-4</v>
       </c>
       <c r="M6" s="37"/>
-      <c r="N6" s="66">
-        <f t="shared" si="2"/>
+      <c r="N6" s="61">
+        <f t="shared" si="3"/>
         <v>1.2634189759030063E-3</v>
       </c>
       <c r="O6" s="5"/>
@@ -2829,20 +2846,20 @@
         <v>0.99734500000000004</v>
       </c>
       <c r="J7" s="59">
+        <f t="shared" si="1"/>
+        <v>3.2321256485970921E-5</v>
+      </c>
+      <c r="K7" s="17">
+        <f t="shared" si="2"/>
+        <v>1.3053253407939462E-3</v>
+      </c>
+      <c r="L7" s="57">
         <f t="shared" si="0"/>
-        <v>3.2321256485970921E-5</v>
-      </c>
-      <c r="K7" s="17">
-        <f t="shared" si="1"/>
-        <v>1.3053253407939462E-3</v>
-      </c>
-      <c r="L7" s="57">
-        <f>C7-(E7)</f>
         <v>1.214141E-2</v>
       </c>
       <c r="M7" s="37"/>
-      <c r="N7" s="66">
-        <f t="shared" si="2"/>
+      <c r="N7" s="61">
+        <f t="shared" si="3"/>
         <v>1.4811732664745309E-3</v>
       </c>
       <c r="O7" s="5"/>
@@ -2879,20 +2896,20 @@
         <v>0.999973</v>
       </c>
       <c r="J8" s="59">
+        <f t="shared" si="1"/>
+        <v>7.9937902023500256E-7</v>
+      </c>
+      <c r="K8" s="17">
+        <f t="shared" si="2"/>
+        <v>1.5434604811577842E-3</v>
+      </c>
+      <c r="L8" s="57">
         <f t="shared" si="0"/>
-        <v>7.9937902023500256E-7</v>
-      </c>
-      <c r="K8" s="17">
-        <f t="shared" si="1"/>
-        <v>1.5434604811577842E-3</v>
-      </c>
-      <c r="L8" s="57">
-        <f>C8-(E8)</f>
         <v>2.9605831000000003E-2</v>
       </c>
       <c r="M8" s="37"/>
-      <c r="N8" s="66">
-        <f t="shared" si="2"/>
+      <c r="N8" s="61">
+        <f t="shared" si="3"/>
         <v>1.6947773472925046E-3</v>
       </c>
       <c r="O8" s="5"/>
@@ -2929,20 +2946,20 @@
         <v>0.999969</v>
       </c>
       <c r="J9" s="59">
+        <f t="shared" si="1"/>
+        <v>6.3791117724695982E-7</v>
+      </c>
+      <c r="K9" s="17">
+        <f t="shared" si="2"/>
+        <v>2.0380616879995734E-3</v>
+      </c>
+      <c r="L9" s="57">
         <f t="shared" si="0"/>
-        <v>6.3791117724695982E-7</v>
-      </c>
-      <c r="K9" s="17">
-        <f t="shared" si="1"/>
-        <v>2.0380616879995734E-3</v>
-      </c>
-      <c r="L9" s="57">
-        <f>C9-(E9)</f>
         <v>2.0577142E-2</v>
       </c>
       <c r="M9" s="37"/>
-      <c r="N9" s="66">
-        <f t="shared" si="2"/>
+      <c r="N9" s="61">
+        <f t="shared" si="3"/>
         <v>2.1549235355556519E-3</v>
       </c>
       <c r="O9" s="5"/>
@@ -2979,20 +2996,20 @@
         <v>1</v>
       </c>
       <c r="J10" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="17">
+        <f t="shared" si="2"/>
+        <v>3.9378616402235365E-3</v>
+      </c>
+      <c r="L10" s="57">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K10" s="17">
-        <f t="shared" si="1"/>
-        <v>3.9378616402235365E-3</v>
-      </c>
-      <c r="L10" s="57">
-        <f>C10-(E10)</f>
         <v>1.952862E-2</v>
       </c>
       <c r="M10" s="37"/>
-      <c r="N10" s="66">
-        <f t="shared" si="2"/>
+      <c r="N10" s="61">
+        <f t="shared" si="3"/>
         <v>3.999594266615553E-3</v>
       </c>
       <c r="O10" s="5"/>

</xml_diff>

<commit_message>
Propogated the correction the parton M_Inv to the trigger bias correction and corresponding systematic
</commit_message>
<xml_diff>
--- a/Sheets/DiJet-EEWW.xlsx
+++ b/Sheets/DiJet-EEWW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/Run15/DijetAsymmetryAnalysis/DijetALLCode/Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EF8996-92AA-8E40-AB4D-5D2CBE53D15C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0545D956-C56E-CC4E-BEC5-085BF5F5E795}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-20400" windowWidth="24000" windowHeight="38400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-19940" windowWidth="24000" windowHeight="37940" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scale - EEWW" sheetId="12" r:id="rId1"/>
@@ -1003,6 +1003,8 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="388" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="386" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1018,8 +1020,6 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="391" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="388" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="392">
     <cellStyle name="20% - Accent2" xfId="388" builtinId="34"/>
@@ -1759,8 +1759,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G10"/>
+    <sheetView showRuler="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1776,24 +1776,24 @@
   <sheetData>
     <row r="1" spans="1:19" ht="26">
       <c r="A1" s="29"/>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
       <c r="R1" s="29"/>
     </row>
     <row r="2" spans="1:19">
@@ -2354,10 +2354,10 @@
       <c r="S13" s="3"/>
     </row>
     <row r="14" spans="1:19">
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="63"/>
+      <c r="C14" s="65"/>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
@@ -2404,8 +2404,8 @@
       <c r="C16" s="13">
         <v>1.1628000000000001</v>
       </c>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
       <c r="G16" s="21"/>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
@@ -2426,8 +2426,8 @@
       <c r="C17" s="13">
         <v>0.81</v>
       </c>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
       <c r="G17" s="21"/>
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
@@ -2448,8 +2448,8 @@
       <c r="C18" s="13">
         <v>0.72</v>
       </c>
-      <c r="E18" s="67"/>
-      <c r="F18" s="67"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
       <c r="Q18" s="11"/>
     </row>
     <row r="19" spans="2:19">
@@ -2459,8 +2459,8 @@
       <c r="C19" s="13">
         <v>0.32</v>
       </c>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -2475,8 +2475,8 @@
       <c r="C20" s="13">
         <v>0.06</v>
       </c>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="15" t="s">
@@ -2485,8 +2485,8 @@
       <c r="C21" s="13">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
     </row>
     <row r="22" spans="2:19" ht="17" thickBot="1">
       <c r="B22" s="16" t="s">
@@ -2495,12 +2495,12 @@
       <c r="C22" s="14">
         <v>0.01</v>
       </c>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
     </row>
     <row r="23" spans="2:19">
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
     </row>
     <row r="24" spans="2:19">
       <c r="E24" s="4"/>
@@ -2560,8 +2560,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AV25"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K10"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2583,19 +2583,19 @@
   <sheetData>
     <row r="1" spans="1:31" ht="22" customHeight="1">
       <c r="A1" s="29"/>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
       <c r="M1" s="29"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -2681,7 +2681,7 @@
         <v>3.565E-3</v>
       </c>
       <c r="E4" s="50">
-        <v>1.75431E-3</v>
+        <v>1.10833E-3</v>
       </c>
       <c r="F4" s="38">
         <v>4.8046100000000001E-4</v>
@@ -2690,27 +2690,27 @@
         <v>6.5789699999999995E-4</v>
       </c>
       <c r="H4" s="38">
-        <v>5.1137899999999996E-4</v>
+        <v>3.1866799999999998E-4</v>
       </c>
       <c r="I4" s="56">
         <v>0.99982599999999999</v>
       </c>
       <c r="J4" s="59">
         <f>((1/I4)-1)*L4</f>
-        <v>1.1259219704228761E-6</v>
+        <v>1.2383420515169887E-6</v>
       </c>
       <c r="K4" s="17">
         <f>SQRT(H4^2 +G4^2 +F4^2 +J4^2)</f>
-        <v>9.6186328782799655E-4</v>
+        <v>8.7476971989491989E-4</v>
       </c>
       <c r="L4" s="57">
         <f t="shared" ref="L4:L10" si="0">C4-(E4)</f>
-        <v>6.4696900000000002E-3</v>
+        <v>7.1156700000000002E-3</v>
       </c>
       <c r="M4" s="37"/>
       <c r="N4" s="61">
         <f>SQRT(K4*K4+E$13*E$13)</f>
-        <v>1.1896137963521116E-3</v>
+        <v>1.1203669322347196E-3</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="7"/>
@@ -2731,7 +2731,7 @@
         <v>2.7650000000000001E-3</v>
       </c>
       <c r="E5" s="50">
-        <v>1.4019E-3</v>
+        <v>5.2214500000000001E-4</v>
       </c>
       <c r="F5" s="38">
         <v>3.4978299999999999E-4</v>
@@ -2740,27 +2740,27 @@
         <v>5.4414800000000005E-4</v>
       </c>
       <c r="H5" s="38">
-        <v>5.9493299999999996E-4</v>
+        <v>3.2945199999999999E-4</v>
       </c>
       <c r="I5" s="56">
         <v>0.999838</v>
       </c>
       <c r="J5" s="59">
         <f t="shared" ref="J5:J10" si="1">((1/I5)-1)*L5</f>
-        <v>6.4795916938550861E-7</v>
+        <v>7.9050257141665265E-7</v>
       </c>
       <c r="K5" s="17">
         <f t="shared" ref="K5:K10" si="2">SQRT(H5^2 +G5^2 +F5^2 +J5^2)</f>
-        <v>8.7885771734285019E-4</v>
+        <v>7.2593693816427017E-4</v>
       </c>
       <c r="L5" s="57">
         <f t="shared" si="0"/>
-        <v>3.9991000000000002E-3</v>
+        <v>4.8788550000000005E-3</v>
       </c>
       <c r="M5" s="37"/>
       <c r="N5" s="61">
         <f t="shared" ref="N5:N10" si="3">SQRT(K5*K5+E$13*E$13)</f>
-        <v>1.1235616971635716E-3</v>
+        <v>1.0084564632106413E-3</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="7"/>
@@ -2781,7 +2781,7 @@
         <v>3.4610000000000001E-3</v>
       </c>
       <c r="E6" s="50">
-        <v>1.05937E-3</v>
+        <v>-1.2275599999999999E-4</v>
       </c>
       <c r="F6" s="38">
         <v>4.7445000000000001E-4</v>
@@ -2790,27 +2790,27 @@
         <v>4.54408E-4</v>
       </c>
       <c r="H6" s="38">
-        <v>8.2136199999999996E-4</v>
+        <v>4.2605600000000001E-4</v>
       </c>
       <c r="I6" s="56">
         <v>0.99704400000000004</v>
       </c>
       <c r="J6" s="59">
         <f t="shared" si="1"/>
-        <v>1.593945984329607E-6</v>
+        <v>5.0986704057190777E-6</v>
       </c>
       <c r="K6" s="17">
         <f t="shared" si="2"/>
-        <v>1.0517735063557178E-3</v>
+        <v>7.8303202012427705E-4</v>
       </c>
       <c r="L6" s="57">
         <f t="shared" si="0"/>
-        <v>5.3762999999999988E-4</v>
+        <v>1.7197559999999998E-3</v>
       </c>
       <c r="M6" s="37"/>
       <c r="N6" s="61">
         <f t="shared" si="3"/>
-        <v>1.2634189759030063E-3</v>
+        <v>1.0503043104452662E-3</v>
       </c>
       <c r="O6" s="5"/>
       <c r="P6" s="7"/>
@@ -2831,7 +2831,7 @@
         <v>5.0600000000000003E-3</v>
       </c>
       <c r="E7" s="50">
-        <v>1.5485900000000001E-3</v>
+        <v>-2.8770300000000001E-5</v>
       </c>
       <c r="F7" s="38">
         <v>6.6018700000000001E-4</v>
@@ -2840,27 +2840,27 @@
         <v>3.7832300000000002E-4</v>
       </c>
       <c r="H7" s="38">
-        <v>1.0601199999999999E-3</v>
+        <v>4.1509099999999997E-4</v>
       </c>
       <c r="I7" s="56">
         <v>0.99734500000000004</v>
       </c>
       <c r="J7" s="59">
         <f t="shared" si="1"/>
-        <v>3.2321256485970921E-5</v>
+        <v>3.6520296533797994E-5</v>
       </c>
       <c r="K7" s="17">
         <f t="shared" si="2"/>
-        <v>1.3053253407939462E-3</v>
+        <v>8.6753065515745111E-4</v>
       </c>
       <c r="L7" s="57">
         <f t="shared" si="0"/>
-        <v>1.214141E-2</v>
+        <v>1.37187703E-2</v>
       </c>
       <c r="M7" s="37"/>
       <c r="N7" s="61">
         <f t="shared" si="3"/>
-        <v>1.4811732664745309E-3</v>
+        <v>1.1147239288890843E-3</v>
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="7"/>
@@ -2881,7 +2881,7 @@
         <v>8.1089999999999999E-3</v>
       </c>
       <c r="E8" s="50">
-        <v>4.4516899999999998E-4</v>
+        <v>-1.5694000000000001E-3</v>
       </c>
       <c r="F8" s="38">
         <v>9.2922000000000002E-4</v>
@@ -2890,27 +2890,27 @@
         <v>3.2183299999999999E-4</v>
       </c>
       <c r="H8" s="38">
-        <v>1.1896400000000001E-3</v>
+        <v>5.7260600000000003E-4</v>
       </c>
       <c r="I8" s="56">
         <v>0.999973</v>
       </c>
       <c r="J8" s="59">
         <f t="shared" si="1"/>
-        <v>7.9937902023500256E-7</v>
+        <v>8.5377385189555639E-7</v>
       </c>
       <c r="K8" s="17">
         <f t="shared" si="2"/>
-        <v>1.5434604811577842E-3</v>
+        <v>1.1379387718391488E-3</v>
       </c>
       <c r="L8" s="57">
         <f t="shared" si="0"/>
-        <v>2.9605831000000003E-2</v>
+        <v>3.16204E-2</v>
       </c>
       <c r="M8" s="37"/>
       <c r="N8" s="61">
         <f t="shared" si="3"/>
-        <v>1.6947773472925046E-3</v>
+        <v>1.3360032366932313E-3</v>
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="7"/>
@@ -2931,7 +2931,7 @@
         <v>1.2102999999999999E-2</v>
       </c>
       <c r="E9" s="50">
-        <v>-5.3214199999999999E-4</v>
+        <v>-3.1687899999999999E-3</v>
       </c>
       <c r="F9" s="38">
         <v>1.03648E-3</v>
@@ -2940,27 +2940,27 @@
         <v>2.7361900000000001E-4</v>
       </c>
       <c r="H9" s="38">
-        <v>1.73336E-3</v>
+        <v>1.1079799999999999E-3</v>
       </c>
       <c r="I9" s="56">
         <v>0.999969</v>
       </c>
       <c r="J9" s="59">
         <f t="shared" si="1"/>
-        <v>6.3791117724695982E-7</v>
+        <v>7.1964979914429839E-7</v>
       </c>
       <c r="K9" s="17">
         <f t="shared" si="2"/>
-        <v>2.0380616879995734E-3</v>
+        <v>1.5416803643611839E-3</v>
       </c>
       <c r="L9" s="57">
         <f t="shared" si="0"/>
-        <v>2.0577142E-2</v>
+        <v>2.3213790000000002E-2</v>
       </c>
       <c r="M9" s="37"/>
       <c r="N9" s="61">
         <f t="shared" si="3"/>
-        <v>2.1549235355556519E-3</v>
+        <v>1.6931563264674743E-3</v>
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="7"/>
@@ -2981,7 +2981,7 @@
         <v>4.1832000000000001E-2</v>
       </c>
       <c r="E10" s="50">
-        <v>-5.8756199999999998E-3</v>
+        <v>-9.1737999999999993E-3</v>
       </c>
       <c r="F10" s="38">
         <v>2.12853E-3</v>
@@ -2990,7 +2990,7 @@
         <v>2.3663800000000001E-4</v>
       </c>
       <c r="H10" s="38">
-        <v>3.3045599999999998E-3</v>
+        <v>2.5395399999999999E-3</v>
       </c>
       <c r="I10" s="56">
         <v>1</v>
@@ -3001,16 +3001,16 @@
       </c>
       <c r="K10" s="17">
         <f t="shared" si="2"/>
-        <v>3.9378616402235365E-3</v>
+        <v>3.322032648175511E-3</v>
       </c>
       <c r="L10" s="57">
         <f t="shared" si="0"/>
-        <v>1.952862E-2</v>
+        <v>2.2826800000000001E-2</v>
       </c>
       <c r="M10" s="37"/>
       <c r="N10" s="61">
         <f t="shared" si="3"/>
-        <v>3.999594266615553E-3</v>
+        <v>3.3949817253623028E-3</v>
       </c>
       <c r="O10" s="5"/>
       <c r="P10" s="7"/>

</xml_diff>